<commit_message>
add qa-preview label ea9bd963e1e8fd522788b03612392cfc76171bd3
</commit_message>
<xml_diff>
--- a/sd-modif-prep-publication-0-4-0-draft/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/sd-modif-prep-publication-0-4-0-draft/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.4.0-ballot-1</t>
+    <t>0.4.0-qa-preview-1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-16T08:11:24+00:00</t>
+    <t>2024-05-16T08:29:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>